<commit_message>
vat bill of lab report for bindabasini mandir
</commit_message>
<xml_diff>
--- a/ofc/estimates/बिन्ध्यबासिनी मन्दिर जाने सडक ढलान/v.xlsx
+++ b/ofc/estimates/बिन्ध्यबासिनी मन्दिर जाने सडक ढलान/v.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">measure!$A$1:$K$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Valuation!$A$1:$K$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">WCR!$A$1:$K$29</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">measure!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">Valuation!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">WCR!$1:$12</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -597,23 +599,8 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -625,6 +612,51 @@
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -633,36 +665,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1324,113 +1326,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:19" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="A2" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -2070,11 +2072,11 @@
       <c r="B36" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="73">
+      <c r="C36" s="68">
         <f>J34</f>
         <v>226120.14918209484</v>
       </c>
-      <c r="D36" s="73"/>
+      <c r="D36" s="68"/>
       <c r="E36" s="21">
         <v>100</v>
       </c>
@@ -2090,10 +2092,10 @@
       <c r="B37" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="76">
+      <c r="C37" s="71">
         <v>200000</v>
       </c>
-      <c r="D37" s="76"/>
+      <c r="D37" s="71"/>
       <c r="E37" s="21"/>
       <c r="F37" s="44"/>
       <c r="G37" s="45"/>
@@ -2107,11 +2109,11 @@
       <c r="B38" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="76">
+      <c r="C38" s="71">
         <f>C37-C40-C41</f>
         <v>190000</v>
       </c>
-      <c r="D38" s="76"/>
+      <c r="D38" s="71"/>
       <c r="E38" s="21">
         <f>C38/C36*100</f>
         <v>84.026125352939147</v>
@@ -2128,11 +2130,11 @@
       <c r="B39" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="73">
+      <c r="C39" s="68">
         <f>C36-C38</f>
         <v>36120.149182094843</v>
       </c>
-      <c r="D39" s="73"/>
+      <c r="D39" s="68"/>
       <c r="E39" s="21">
         <f>100-E38</f>
         <v>15.973874647060853</v>
@@ -2149,11 +2151,11 @@
       <c r="B40" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="73">
+      <c r="C40" s="68">
         <f>C37*0.03</f>
         <v>6000</v>
       </c>
-      <c r="D40" s="73"/>
+      <c r="D40" s="68"/>
       <c r="E40" s="21">
         <v>3</v>
       </c>
@@ -2169,11 +2171,11 @@
       <c r="B41" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="73">
+      <c r="C41" s="68">
         <f>C37*0.02</f>
         <v>4000</v>
       </c>
-      <c r="D41" s="73"/>
+      <c r="D41" s="68"/>
       <c r="E41" s="21">
         <v>2</v>
       </c>
@@ -2186,6 +2188,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="A7:F7"/>
@@ -2194,13 +2203,6 @@
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2211,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,113 +2231,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="A2" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -3434,11 +3436,11 @@
         <v>33</v>
       </c>
       <c r="I51" s="14">
-        <v>15000</v>
+        <v>14999</v>
       </c>
       <c r="J51" s="36">
         <f>G51*I51</f>
-        <v>15000</v>
+        <v>14999</v>
       </c>
       <c r="K51" s="13"/>
       <c r="M51" s="17"/>
@@ -3532,7 +3534,7 @@
       <c r="I55" s="16"/>
       <c r="J55" s="16">
         <f>SUM(J18:J53)</f>
-        <v>228081.1803271111</v>
+        <v>228080.1803271111</v>
       </c>
       <c r="K55" s="19"/>
     </row>
@@ -3541,11 +3543,11 @@
       <c r="B57" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="73">
+      <c r="C57" s="68">
         <f>J55</f>
-        <v>228081.1803271111</v>
-      </c>
-      <c r="D57" s="73"/>
+        <v>228080.1803271111</v>
+      </c>
+      <c r="D57" s="68"/>
       <c r="E57" s="21">
         <v>100</v>
       </c>
@@ -3561,10 +3563,10 @@
       <c r="B58" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="76">
+      <c r="C58" s="71">
         <v>200000</v>
       </c>
-      <c r="D58" s="76"/>
+      <c r="D58" s="71"/>
       <c r="E58" s="21"/>
       <c r="F58" s="44"/>
       <c r="G58" s="45"/>
@@ -3578,14 +3580,14 @@
       <c r="B59" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="76">
+      <c r="C59" s="71">
         <f>C58-C61-C62</f>
         <v>190000</v>
       </c>
-      <c r="D59" s="76"/>
+      <c r="D59" s="71"/>
       <c r="E59" s="21">
         <f>C59/C57*100</f>
-        <v>83.303672721924897</v>
+        <v>83.304037960467781</v>
       </c>
       <c r="F59" s="44"/>
       <c r="G59" s="45"/>
@@ -3599,14 +3601,14 @@
       <c r="B60" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="73">
+      <c r="C60" s="68">
         <f>C57-C59</f>
-        <v>38081.180327111098</v>
-      </c>
-      <c r="D60" s="73"/>
+        <v>38080.180327111098</v>
+      </c>
+      <c r="D60" s="68"/>
       <c r="E60" s="21">
         <f>100-E59</f>
-        <v>16.696327278075103</v>
+        <v>16.695962039532219</v>
       </c>
       <c r="F60" s="44"/>
       <c r="G60" s="45"/>
@@ -3620,11 +3622,11 @@
       <c r="B61" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="73">
+      <c r="C61" s="68">
         <f>C58*0.03</f>
         <v>6000</v>
       </c>
-      <c r="D61" s="73"/>
+      <c r="D61" s="68"/>
       <c r="E61" s="21">
         <v>3</v>
       </c>
@@ -3640,11 +3642,11 @@
       <c r="B62" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="73">
+      <c r="C62" s="68">
         <f>C58*0.02</f>
         <v>4000</v>
       </c>
-      <c r="D62" s="73"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="21">
         <v>2</v>
       </c>
@@ -3657,6 +3659,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="A7:F7"/>
@@ -3665,13 +3674,6 @@
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -3837,14 +3839,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:F8"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -3858,90 +3860,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="85" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
+      <c r="A2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="52" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="52"/>
-      <c r="C6" s="87">
+      <c r="C6" s="78">
         <f>F29</f>
         <v>226120.14918209484</v>
       </c>
-      <c r="D6" s="88"/>
+      <c r="D6" s="79"/>
       <c r="E6" s="53"/>
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
@@ -3949,11 +3951,11 @@
         <v>55</v>
       </c>
       <c r="I6" s="52"/>
-      <c r="J6" s="87">
+      <c r="J6" s="78">
         <f>I29</f>
-        <v>228081.1803271111</v>
-      </c>
-      <c r="K6" s="88"/>
+        <v>228080.1803271111</v>
+      </c>
+      <c r="K6" s="79"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
@@ -3962,77 +3964,77 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="I7" s="81" t="s">
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="I7" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="str">
+      <c r="A8" s="72" t="str">
         <f>Estimate!A6</f>
         <v>Project:- बिन्ध्यबासिनी मन्दिर जाने सडक ढलान</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="I8" s="82" t="s">
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="I8" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="str">
+      <c r="A9" s="86" t="str">
         <f>Estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="I9" s="82" t="s">
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="I9" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79" t="s">
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="78" t="s">
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="77" t="s">
+      <c r="K11" s="87" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="55" t="s">
         <v>64</v>
       </c>
@@ -4051,10 +4053,10 @@
       <c r="I12" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="78"/>
-      <c r="K12" s="77"/>
-    </row>
-    <row r="13" spans="1:11" s="18" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="J12" s="88"/>
+      <c r="K12" s="87"/>
+    </row>
+    <row r="13" spans="1:11" s="18" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A13" s="66">
         <f>Estimate!A9</f>
         <v>1</v>
@@ -4377,7 +4379,7 @@
       <c r="I24" s="56"/>
       <c r="J24" s="57"/>
       <c r="K24" s="58"/>
-      <c r="M24" s="89"/>
+      <c r="M24" s="67"/>
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="66">
@@ -4410,15 +4412,15 @@
       </c>
       <c r="H25" s="56">
         <f>Valuation!I51</f>
-        <v>15000</v>
+        <v>14999</v>
       </c>
       <c r="I25" s="56">
         <f>G25*H25</f>
-        <v>15000</v>
+        <v>14999</v>
       </c>
       <c r="J25" s="57">
         <f>I25-F25</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K25" s="58"/>
     </row>
@@ -4507,16 +4509,29 @@
       <c r="H29" s="62"/>
       <c r="I29" s="62">
         <f>SUM(I13:I27)</f>
-        <v>228081.1803271111</v>
+        <v>228080.1803271111</v>
       </c>
       <c r="J29" s="63">
         <f>I29-F29</f>
-        <v>1961.0311450162553</v>
+        <v>1960.0311450162553</v>
       </c>
       <c r="K29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -4524,23 +4539,10 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;LPrepared By:
 &amp;CChecked By:
@@ -4554,7 +4556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScale="60" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -4572,113 +4574,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="A2" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -5884,11 +5886,11 @@
       <c r="B57" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="73">
+      <c r="C57" s="68">
         <f>J55</f>
         <v>228081.1803271111</v>
       </c>
-      <c r="D57" s="73"/>
+      <c r="D57" s="68"/>
       <c r="E57" s="21">
         <v>100</v>
       </c>
@@ -5904,10 +5906,10 @@
       <c r="B58" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="76">
+      <c r="C58" s="71">
         <v>200000</v>
       </c>
-      <c r="D58" s="76"/>
+      <c r="D58" s="71"/>
       <c r="E58" s="21"/>
       <c r="F58" s="44"/>
       <c r="G58" s="45"/>
@@ -5921,11 +5923,11 @@
       <c r="B59" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="76">
+      <c r="C59" s="71">
         <f>C58-C61-C62</f>
         <v>190000</v>
       </c>
-      <c r="D59" s="76"/>
+      <c r="D59" s="71"/>
       <c r="E59" s="21">
         <f>C59/C57*100</f>
         <v>83.303672721924897</v>
@@ -5942,11 +5944,11 @@
       <c r="B60" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="73">
+      <c r="C60" s="68">
         <f>C57-C59</f>
         <v>38081.180327111098</v>
       </c>
-      <c r="D60" s="73"/>
+      <c r="D60" s="68"/>
       <c r="E60" s="21">
         <f>100-E59</f>
         <v>16.696327278075103</v>
@@ -5963,11 +5965,11 @@
       <c r="B61" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="73">
+      <c r="C61" s="68">
         <f>C58*0.03</f>
         <v>6000</v>
       </c>
-      <c r="D61" s="73"/>
+      <c r="D61" s="68"/>
       <c r="E61" s="21">
         <v>3</v>
       </c>
@@ -5983,11 +5985,11 @@
       <c r="B62" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="73">
+      <c r="C62" s="68">
         <f>C58*0.02</f>
         <v>4000</v>
       </c>
-      <c r="D62" s="73"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="21">
         <v>2</v>
       </c>
@@ -6000,6 +6002,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="A7:F7"/>
@@ -6008,16 +6017,9 @@
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
   </headerFooter>

</xml_diff>